<commit_message>
20201202(added rows' and columns' names)
</commit_message>
<xml_diff>
--- a/Hospital beds and length of stay.xlsx
+++ b/Hospital beds and length of stay.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kv/Desktop/ESBL and CR strain of Klebsiella pneumoniae in Europe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD0BC19-1824-414F-B21C-003A87675A1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD10031-FA7F-E143-A8E7-A445D8C40D26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{52E54497-8E42-8F47-851F-758485A19451}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19580" xr2:uid="{52E54497-8E42-8F47-851F-758485A19451}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -430,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55BF0604-0973-5A4C-953F-903C243E4CFC}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="A14" sqref="A14:L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -857,397 +857,397 @@
         <v>272.33333333333331</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13">
-        <v>2015</v>
-      </c>
-      <c r="C13">
-        <v>2014</v>
-      </c>
-      <c r="D13">
-        <v>2013</v>
-      </c>
-      <c r="E13">
-        <v>2012</v>
-      </c>
-      <c r="F13">
-        <v>2011</v>
-      </c>
-      <c r="G13">
-        <v>2010</v>
-      </c>
-      <c r="H13">
-        <v>2009</v>
-      </c>
-      <c r="I13">
-        <v>2008</v>
-      </c>
-      <c r="J13">
-        <v>2007</v>
-      </c>
-      <c r="K13">
-        <v>2006</v>
-      </c>
-      <c r="L13">
-        <v>2005</v>
-      </c>
-    </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>2015</v>
       </c>
       <c r="C14">
-        <v>8.8000000000000007</v>
+        <v>2014</v>
       </c>
       <c r="D14">
-        <v>8.9</v>
+        <v>2013</v>
       </c>
       <c r="E14">
-        <v>9.1</v>
+        <v>2012</v>
       </c>
       <c r="F14">
-        <v>9.3000000000000007</v>
+        <v>2011</v>
       </c>
       <c r="G14">
-        <v>9.5</v>
+        <v>2010</v>
       </c>
       <c r="H14">
-        <v>9.6999999999999993</v>
+        <v>2009</v>
       </c>
       <c r="I14">
-        <v>9.6</v>
+        <v>2008</v>
       </c>
       <c r="J14">
-        <v>9.8000000000000007</v>
+        <v>2007</v>
       </c>
       <c r="K14">
-        <v>9.9</v>
+        <v>2006</v>
       </c>
       <c r="L14">
-        <f>AVERAGE(B14:K14)</f>
-        <v>9.4</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>8.8000000000000007</v>
       </c>
       <c r="D15">
-        <v>4.3</v>
+        <v>8.9</v>
       </c>
       <c r="E15">
-        <v>4.4000000000000004</v>
+        <v>9.1</v>
       </c>
       <c r="F15">
-        <v>4.5</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="G15">
-        <v>4.5999999999999996</v>
+        <v>9.5</v>
       </c>
       <c r="H15">
-        <v>4.8</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="I15">
-        <v>5.2</v>
+        <v>9.6</v>
       </c>
       <c r="J15">
-        <v>5.2</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="K15">
-        <v>5.3</v>
+        <v>9.9</v>
       </c>
       <c r="L15">
-        <f t="shared" ref="L15:L24" si="2">AVERAGE(B15:K15)</f>
-        <v>4.7874999999999996</v>
+        <f>AVERAGE(B15:K15)</f>
+        <v>9.4</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>4.3</v>
+      </c>
+      <c r="E16">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F16">
+        <v>4.5</v>
+      </c>
+      <c r="G16">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="H16">
+        <v>4.8</v>
+      </c>
+      <c r="I16">
+        <v>5.2</v>
+      </c>
+      <c r="J16">
+        <v>5.2</v>
+      </c>
+      <c r="K16">
+        <v>5.3</v>
+      </c>
+      <c r="L16">
+        <f t="shared" ref="L16:L25" si="2">AVERAGE(B16:K16)</f>
+        <v>4.7874999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>3</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>10.6</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <v>10.8</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <v>11.2</v>
       </c>
-      <c r="F16">
+      <c r="F17">
         <v>11.4</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <v>11.8</v>
       </c>
-      <c r="H16">
+      <c r="H17">
         <v>12.7</v>
       </c>
-      <c r="I16">
+      <c r="I17">
         <v>12.6</v>
       </c>
-      <c r="J16">
+      <c r="J17">
         <v>13.1</v>
       </c>
-      <c r="K16">
+      <c r="K17">
         <v>12.8</v>
       </c>
-      <c r="L16">
+      <c r="L17">
         <f t="shared" si="2"/>
         <v>11.888888888888888</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>10.1</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>10.1</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <v>10.1</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <v>10.199999999999999</v>
       </c>
-      <c r="H17">
+      <c r="H18">
         <v>10.5</v>
       </c>
-      <c r="I17">
+      <c r="I18">
         <v>10.9</v>
       </c>
-      <c r="J17">
+      <c r="J18">
         <v>11.2</v>
       </c>
-      <c r="K17">
+      <c r="K18">
         <v>11.2</v>
       </c>
-      <c r="L17">
+      <c r="L18">
         <f t="shared" si="2"/>
         <v>10.5375</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>5</v>
       </c>
-      <c r="F18">
+      <c r="F19">
         <v>6.8</v>
       </c>
-      <c r="G18">
+      <c r="G19">
         <v>6.6</v>
       </c>
-      <c r="H18">
+      <c r="H19">
         <v>6.7</v>
       </c>
-      <c r="I18">
+      <c r="I19">
         <v>6.6</v>
       </c>
-      <c r="J18">
+      <c r="J19">
         <v>6.9</v>
       </c>
-      <c r="K18">
+      <c r="K19">
         <v>7.3</v>
       </c>
-      <c r="L18">
+      <c r="L19">
         <f t="shared" si="2"/>
         <v>6.8166666666666655</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>6</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>9.5</v>
       </c>
-      <c r="D19">
+      <c r="D20">
         <v>9.3000000000000007</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <v>9.6</v>
       </c>
-      <c r="F19">
+      <c r="F20">
         <v>9.5</v>
       </c>
-      <c r="G19">
+      <c r="G20">
         <v>9.5</v>
       </c>
-      <c r="H19">
+      <c r="H20">
         <v>9.1999999999999993</v>
       </c>
-      <c r="I19">
+      <c r="I20">
         <v>9.1999999999999993</v>
       </c>
-      <c r="J19">
+      <c r="J20">
         <v>8.9</v>
       </c>
-      <c r="K19">
+      <c r="K20">
         <v>8.6999999999999993</v>
       </c>
-      <c r="L19">
+      <c r="L20">
         <f t="shared" si="2"/>
         <v>9.2666666666666675</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>7</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <v>8</v>
       </c>
-      <c r="D20">
+      <c r="D21">
         <v>7.9</v>
       </c>
-      <c r="E20">
+      <c r="E21">
         <v>8</v>
       </c>
-      <c r="F20">
+      <c r="F21">
         <v>8</v>
       </c>
-      <c r="G20">
+      <c r="G21">
         <v>7.9</v>
       </c>
-      <c r="H20">
+      <c r="H21">
         <v>7.8</v>
       </c>
-      <c r="I20">
+      <c r="I21">
         <v>7.8</v>
       </c>
-      <c r="J20">
+      <c r="J21">
         <v>7.8</v>
       </c>
-      <c r="K20">
+      <c r="K21">
         <v>7.7</v>
       </c>
-      <c r="L20">
+      <c r="L21">
         <f t="shared" si="2"/>
         <v>7.8777777777777764</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>8</v>
       </c>
-      <c r="K21">
+      <c r="K22">
         <v>10.8</v>
       </c>
-      <c r="L21">
+      <c r="L22">
         <f t="shared" si="2"/>
         <v>10.8</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>9</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <v>6</v>
       </c>
-      <c r="D22">
+      <c r="D23">
         <v>6.1</v>
       </c>
-      <c r="E22">
+      <c r="E23">
         <v>6.2</v>
       </c>
-      <c r="F22">
+      <c r="F23">
         <v>6.5</v>
       </c>
-      <c r="G22">
+      <c r="G23">
         <v>6.8</v>
       </c>
-      <c r="H22">
+      <c r="H23">
         <v>7</v>
       </c>
-      <c r="I22">
+      <c r="I23">
         <v>7.3</v>
       </c>
-      <c r="J22">
+      <c r="J23">
         <v>7.6</v>
       </c>
-      <c r="K22">
+      <c r="K23">
         <v>7.7</v>
       </c>
-      <c r="L22">
+      <c r="L23">
         <f t="shared" si="2"/>
         <v>6.8000000000000007</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>10</v>
       </c>
-      <c r="C23">
+      <c r="C24">
         <v>8.9</v>
       </c>
-      <c r="D23">
+      <c r="D24">
         <v>8.9</v>
       </c>
-      <c r="E23">
+      <c r="E24">
         <v>9</v>
       </c>
-      <c r="F23">
+      <c r="F24">
         <v>8.6999999999999993</v>
       </c>
-      <c r="G23">
+      <c r="G24">
         <v>8.6999999999999993</v>
       </c>
-      <c r="H23">
+      <c r="H24">
         <v>8.6</v>
       </c>
-      <c r="I23">
+      <c r="I24">
         <v>8.4</v>
       </c>
-      <c r="J23">
+      <c r="J24">
         <v>8.5</v>
       </c>
-      <c r="K23">
+      <c r="K24">
         <v>8.6</v>
       </c>
-      <c r="L23">
+      <c r="L24">
         <f t="shared" si="2"/>
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>11</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <v>5.7</v>
       </c>
-      <c r="D24">
+      <c r="D25">
         <v>5.8</v>
       </c>
-      <c r="E24">
+      <c r="E25">
         <v>5.8</v>
       </c>
-      <c r="F24">
+      <c r="F25">
         <v>5.9</v>
       </c>
-      <c r="G24">
+      <c r="G25">
         <v>6.1</v>
       </c>
-      <c r="H24">
+      <c r="H25">
         <v>6.4</v>
       </c>
-      <c r="I24">
+      <c r="I25">
         <v>6.5</v>
       </c>
-      <c r="J24">
+      <c r="J25">
         <v>6.5</v>
       </c>
-      <c r="K24">
+      <c r="K25">
         <v>6.6</v>
       </c>
-      <c r="L24">
+      <c r="L25">
         <f t="shared" si="2"/>
         <v>6.1444444444444448</v>
       </c>

</xml_diff>